<commit_message>
Unit supporting - millimeter, inch
AGM.Modelling.SaveSat, AGM.Modelling.ExportFile can export file with millimeter, inch;
AGM.Modelling.ImportFile can import file with millimeter, inch
</commit_message>
<xml_diff>
--- a/修改日志.xlsx
+++ b/修改日志.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="154">
   <si>
     <t>日期</t>
   </si>
@@ -435,9 +435,6 @@
     <t>filepath：SAT文件路径</t>
   </si>
   <si>
-    <t>AGM.Modelling.SaveSat(filepath, version=-1)</t>
-  </si>
-  <si>
     <t>version:  SAT文件版本号，可以输入数字，比如16就代表16版本的Sat
 如果不设置version就是当前的Sat版本，当前的版本是28</t>
   </si>
@@ -460,32 +457,6 @@
   </si>
   <si>
     <t>filepath：导出的Step、Iges文件</t>
-  </si>
-  <si>
-    <r>
-      <t>AGM.Modelling.ExportFile(filepath, logpath)
-可以导出Step、Iges文件（</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>保存Sat用AGM.Modelling.SaveSat</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
   </si>
   <si>
     <t>equation_x\equation_y\equation_z: 字符串形式的线方程的三个分量
@@ -966,6 +937,89 @@
   </si>
   <si>
     <t>vertex | array of vertex : 一个点或者一组点, 得到连接在同一个vertex上的所有的edge</t>
+  </si>
+  <si>
+    <t>unit:
+单位，字符串，目前支持"millimeter"和"inch"
+如果用户不设置unit，默认是"millimeter"</t>
+  </si>
+  <si>
+    <t>product_id:
+SAT文件作者，字符串
+如果用户不设置product_id，默认是"This model is generated by MiSUMi Corporation.Copyright@MiSUMi"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>新增：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+AGM.Modelling.SaveSat
+//AGM.Modelling.SaveSat( filepath, version, unit, product_id )
+保存时可以设置SAT文件的版本号，SAT文件的单位，SAT文件的作者
+（命令参数参考js_files\radf_init.js，命令使用参考js_files\Export.js）
+AGM.Modelling.ExportFile
+//AGM.Modelling.ExportFile( filepath, unit, logpath )
+保存时可以设置文件（SAT、STEP、IGES）的单位
+（命令参数参考js_files\radf_init.js，命令使用参考js_files\Export.js）
+AGM.Modelling.ImportFile
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>这个命令的接口没有变，但是内部支持单位的转换；因为SID.exe默认的单位是mm，所以无论导入的模型（SAT、STEP、IGES）本身的单位是什么（millimeter, inch），该命令都会自动转换成mm，同时根据需要调整模型</t>
+    </r>
+  </si>
+  <si>
+    <t>AGM.Modelling.SaveSat(filepath, version=-1, unit="millimeter", product_id="This model is generated by MiSUMi Corporation.Copyright@MiSUMi")
+范例：Export.js</t>
+  </si>
+  <si>
+    <r>
+      <t>AGM.Modelling.ExportFile(filepath,  unit, logpath)
+可以导出Step、Iges文件（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>保存Sat用AGM.Modelling.SaveSat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+范例：Export.js</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1601,10 +1655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1706,7 +1760,7 @@
         <v>20181011</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="105">
@@ -1714,7 +1768,7 @@
         <v>20181030</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="105">
@@ -1722,7 +1776,7 @@
         <v>20181031</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="105">
@@ -1730,7 +1784,7 @@
         <v>20181105</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="60">
@@ -1738,7 +1792,7 @@
         <v>20181107</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="120">
@@ -1746,7 +1800,7 @@
         <v>20181129</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="315">
@@ -1754,7 +1808,7 @@
         <v>20181205</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="45">
@@ -1762,7 +1816,15 @@
         <v>20181208</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="225">
+      <c r="A20" s="1">
+        <v>20181228</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1775,8 +1837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H80" sqref="H80"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2304,21 +2366,25 @@
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
     </row>
-    <row r="30" spans="1:11" ht="75">
+    <row r="30" spans="1:11" ht="150">
       <c r="A30" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>64</v>
+        <v>152</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
+        <v>64</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>150</v>
+      </c>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
@@ -2330,13 +2396,13 @@
         <v>6</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="D31" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
@@ -2346,20 +2412,22 @@
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
     </row>
-    <row r="32" spans="1:11" ht="45">
+    <row r="32" spans="1:11" ht="75">
       <c r="A32" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>71</v>
+        <v>153</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E32" s="4"/>
+        <v>149</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
@@ -2372,25 +2440,25 @@
         <v>6</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C33" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H33" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="H33" s="8" t="s">
-        <v>75</v>
       </c>
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
@@ -2401,19 +2469,19 @@
         <v>6</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C34" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E34" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="F34" s="9" t="s">
         <v>80</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>82</v>
       </c>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
@@ -2426,13 +2494,13 @@
         <v>6</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
@@ -2447,24 +2515,24 @@
         <v>6</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C36" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E36" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>90</v>
-      </c>
       <c r="F36" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
@@ -2474,19 +2542,19 @@
         <v>6</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
@@ -2499,25 +2567,25 @@
         <v>6</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D38" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E38" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="F38" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="G38" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="G38" s="11" t="s">
-        <v>102</v>
-      </c>
       <c r="H38" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I38" s="11"/>
       <c r="J38" s="10"/>
@@ -2528,28 +2596,28 @@
         <v>6</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C39" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E39" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="F39" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="G39" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="F39" s="11" t="s">
+      <c r="H39" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="G39" s="11" t="s">
+      <c r="I39" s="11" t="s">
         <v>107</v>
-      </c>
-      <c r="H39" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="I39" s="11" t="s">
-        <v>109</v>
       </c>
       <c r="J39" s="11"/>
       <c r="K39" s="11"/>
@@ -2832,16 +2900,16 @@
         <v>6</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
@@ -2855,16 +2923,16 @@
         <v>6</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C62" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D62" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E62" s="11" t="s">
         <v>120</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="E62" s="11" t="s">
-        <v>122</v>
       </c>
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
@@ -2878,13 +2946,13 @@
         <v>6</v>
       </c>
       <c r="B63" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D63" s="5" t="s">
         <v>124</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>126</v>
       </c>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
@@ -2899,10 +2967,10 @@
         <v>6</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
@@ -2918,7 +2986,7 @@
         <v>6</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
@@ -2935,13 +3003,13 @@
         <v>6</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C66" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D66" s="5" t="s">
         <v>131</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>133</v>
       </c>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
@@ -2953,10 +3021,10 @@
     </row>
     <row r="67" spans="1:11" ht="45">
       <c r="A67" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>14</v>
@@ -2976,13 +3044,13 @@
     </row>
     <row r="68" spans="1:11" ht="30">
       <c r="A68" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C68" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>139</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
@@ -2998,13 +3066,13 @@
         <v>6</v>
       </c>
       <c r="B69" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D69" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>142</v>
       </c>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
@@ -3019,13 +3087,13 @@
         <v>6</v>
       </c>
       <c r="B70" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D70" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>145</v>
       </c>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
@@ -3037,16 +3105,16 @@
     </row>
     <row r="71" spans="1:11" ht="75">
       <c r="A71" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>

</xml_diff>

<commit_message>
Support inch as input unit
AGM.Modelling.ScalePart( scale ); AGM.Modelling.ScaleBody( body, scale )
</commit_message>
<xml_diff>
--- a/修改日志.xlsx
+++ b/修改日志.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="159">
   <si>
     <t>日期</t>
   </si>
@@ -1020,6 +1020,48 @@
       <t>）
 范例：Export.js</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>新增：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+AGM.Modelling.ScalePart
+//AGM.Modelling.ScalePart( scale )
+缩放整个零件文档里面所有的body
+AGM.Modelling.ScaleBody = modellingScaleBody
+//AGM.Modelling.ScaleBody( body, scale )
+缩放指定的body</t>
+    </r>
+  </si>
+  <si>
+    <t>AGM.Modelling.ScalePart( scale )
+缩放整个零件文档里面所有的body</t>
+  </si>
+  <si>
+    <t>AGM.Modelling.ScaleBody( body, scale )
+缩放指定的body</t>
+  </si>
+  <si>
+    <t>scale : double类型，缩放比例</t>
+  </si>
+  <si>
+    <t>body : 指定的body对象</t>
   </si>
 </sst>
 </file>
@@ -1330,15 +1372,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>99390</xdr:colOff>
+      <xdr:colOff>207064</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>217118</xdr:rowOff>
+      <xdr:rowOff>183987</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1481</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>9144</xdr:rowOff>
+      <xdr:colOff>109155</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>166513</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1355,7 +1397,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13641455" y="31020140"/>
+          <a:off x="13749129" y="32320509"/>
           <a:ext cx="4300156" cy="3411526"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1655,10 +1697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1827,6 +1869,14 @@
         <v>151</v>
       </c>
     </row>
+    <row r="21" spans="1:2" ht="120">
+      <c r="A21" s="1">
+        <v>20181228</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1835,10 +1885,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K71"/>
+  <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3123,6 +3173,46 @@
       <c r="I71" s="5"/>
       <c r="J71" s="5"/>
       <c r="K71" s="5"/>
+    </row>
+    <row r="72" spans="1:11" ht="30">
+      <c r="A72" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
+      <c r="I72" s="5"/>
+      <c r="J72" s="5"/>
+      <c r="K72" s="5"/>
+    </row>
+    <row r="73" spans="1:11" ht="30">
+      <c r="A73" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
+      <c r="H73" s="5"/>
+      <c r="I73" s="5"/>
+      <c r="J73" s="5"/>
+      <c r="K73" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
New commands : Sweep and Combine\Separate
//AGM.Sketcher.ConvertToPath( DoGSketch, out WireObject)
AGM.Sketcher.ConvertToPath = sketchConvertToPath;

//AGM.Modelling.Combine( blank, tool0, tool1, tool2...)
AGM.Modelling.Combine = modellingCombine;

//AGM.Modelling.Separate( ModelObject, out Array of ModelObject)
AGM.Modelling.Separate = modellingSeparate;
</commit_message>
<xml_diff>
--- a/修改日志.xlsx
+++ b/修改日志.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="修改记录" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="170">
   <si>
     <t>日期</t>
   </si>
@@ -1062,6 +1062,152 @@
   </si>
   <si>
     <t>body : 指定的body对象</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">升级：
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Acis\IOP从R2018.1.1.0升级到R2019.1.0.0 HF9
+Bugfix : Acis sweep with draft [Incident: 181129-000002]</t>
+    </r>
+  </si>
+  <si>
+    <t>AGM.Sketcher.ConvertToPath( DoGSketch, out WireObject)
+将草图轮廓转换为扫略路径
+范例:SweepCut.js\SweepCut_2.js</t>
+  </si>
+  <si>
+    <t>out WireObject : 生成的扫略路径</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AGM.Modelling.Combine( blank, tool0, tool1, tool2...)
+将所有的body（blank, tool0 - tooln）合并到blank上
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>注意：所有的body必须是互不相交的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+范例:Combine&amp;Separate.js</t>
+    </r>
+  </si>
+  <si>
+    <t>blank : 所有的body都合并到输入的blank body上</t>
+  </si>
+  <si>
+    <t>tool0 - tooln: 待合并的body，数量可以任意多</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">修改：
+AGM.Modelling.Sweep名称修改为AGM.Modelling.SweepByPath
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>新增：
+AGM.Sketcher.ConvertToPath</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+//AGM.Sketcher.ConvertToPath( DoGSketch, out WireObject)
+（命令参数参考js_files\radf_init.js，命令使用参考js_files\SweepCut.js, SweepCut_2.js）</t>
+    </r>
+  </si>
+  <si>
+    <t>out Array of ModelObject : 输入是一个空的数组，拆分出来的body放到数组中输出</t>
+  </si>
+  <si>
+    <t>ModelObject : 输入的待拆分的body</t>
+  </si>
+  <si>
+    <t>AGM.Modelling.Separate( ModelObject, out Array of ModelObject)
+如果ModelObject内部包含不相连的几块，则将每块都转成一个body；如果ModelObjec本身只有一块，那么输出的数组就只包含输入的ModelObjec一个body
+范例:Combine&amp;Separate.js</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>新增：
+AGM.Modelling.Combine</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+//AGM.Modelling.Combine( blank, tool0, tool1, tool2...)
+（命令参数参考js_files\radf_init.js，命令使用参考js_files\Combine&amp;Separate.js）
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">AGM.Modelling.Separate
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>//AGM.Modelling.Separate( ModelObject, out Array of ModelObject)
+（命令参数参考js_files\radf_init.js，命令使用参考js_files\Combine&amp;Separate.js）</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1163,7 +1309,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1195,6 +1341,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1379,8 +1528,8 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>109155</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>166513</xdr:rowOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>357013</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1697,10 +1846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1877,6 +2026,30 @@
         <v>154</v>
       </c>
     </row>
+    <row r="22" spans="1:2" ht="45">
+      <c r="A22" s="1">
+        <v>20180213</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="90">
+      <c r="A23" s="1">
+        <v>20180221</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="105">
+      <c r="A24" s="1">
+        <v>20180222</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1885,10 +2058,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K73"/>
+  <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView topLeftCell="A70" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1910,17 +2083,17 @@
       <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:11" ht="70.5" customHeight="1">
       <c r="A2" s="5" t="s">
@@ -3213,6 +3386,69 @@
       <c r="I73" s="5"/>
       <c r="J73" s="5"/>
       <c r="K73" s="5"/>
+    </row>
+    <row r="74" spans="1:11" ht="45">
+      <c r="A74" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5"/>
+      <c r="I74" s="5"/>
+      <c r="J74" s="5"/>
+      <c r="K74" s="5"/>
+    </row>
+    <row r="75" spans="1:11" ht="60">
+      <c r="A75" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5"/>
+      <c r="J75" s="5"/>
+      <c r="K75" s="5"/>
+    </row>
+    <row r="76" spans="1:11" ht="90">
+      <c r="A76" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="5"/>
+      <c r="J76" s="5"/>
+      <c r="K76" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Support to pick face\edge\vertex on input body
AGM.Modelling.PickFace支持从特定body上选择面
//AGM.Modelling.PickFace( point, vector, apertureb, body)
AGM.Modelling.PickEdge支持从特定body上选择边
//AGM.Modelling.PickEdge( point, vector, apertureb, body)
AGM.Modelling.PickVertex支持从特定body上选择顶点
//AGM.Modelling.PickVertex( point, vector, apertureb, body)
</commit_message>
<xml_diff>
--- a/修改日志.xlsx
+++ b/修改日志.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="181">
   <si>
     <t>日期</t>
   </si>
@@ -164,14 +164,6 @@
   </si>
   <si>
     <t>AGM.Modelling.SetEntityColor( entity|Array of entities, r, g, b )</t>
-  </si>
-  <si>
-    <t>AGM.Modelling.PickEdge( point, vector, apertureb)
-范例：blend.js\chamfer1.js\chamfer2.js</t>
-  </si>
-  <si>
-    <t>AGM.Modelling.PickFace( point, vector, apertureb)
-范例：chamfer2.js</t>
   </si>
   <si>
     <t>AGM.Modelling.ChamferEdge( edge|Array of edges, left_range, left_face, right_range)
@@ -1252,6 +1244,74 @@
     <t>AGM.Modelling.ConvertFaceToPath( face, out WireObject )
 提取face最外层的轮廓生成扫略路径
 范例:SweepCut_3.js</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>修改：
+AGM.Modelling.PickFace支持从特定body上选择面
+//AGM.Modelling.PickFace( point, vector, apertureb, body)
+AGM.Modelling.PickEdge支持从特定body上选择边
+//AGM.Modelling.PickEdge( point, vector, apertureb, body)
+AGM.Modelling.PickVertex支持从特定body上选择顶点
+//AGM.Modelling.PickVertex( point, vector, apertureb, body)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>object : 成功返回face对象；失败返回null</t>
+  </si>
+  <si>
+    <t>AGM.Modelling.PickEdge( point, vector, apertureb, body)
+范例：blend.js\chamfer1.js\chamfer2.js</t>
+  </si>
+  <si>
+    <t>AGM.Modelling.PickFace( point, vector, apertureb, body)
+范例：chamfer2.js</t>
+  </si>
+  <si>
+    <t>object : 成功返回Vertex对象；失败返回null</t>
+  </si>
+  <si>
+    <t>AGM.Modelling.PickVertex( point, vector, apertureb, body)</t>
+  </si>
+  <si>
+    <t>body : 如果有，表示从特定的body上选择面</t>
+  </si>
+  <si>
+    <t>body : 如果有，表示从特定的body上选择边</t>
+  </si>
+  <si>
+    <t>body : 如果有，表示从特定的body上选择顶点</t>
+  </si>
+  <si>
+    <t>AGM.Modelling.BlendEdge( edge|Array of edges, radius )
+范例：chamfer2.js</t>
   </si>
 </sst>
 </file>
@@ -1353,7 +1413,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1392,6 +1452,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1414,13 +1477,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2685724</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>171183</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1452,13 +1515,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>602526</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>165653</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>268553</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>127297</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1490,13 +1553,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>196802</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>140805</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>960782</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>131293</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1528,13 +1591,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>41413</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>304954</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>957119</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>1656522</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1566,13 +1629,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>207064</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>183987</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>109155</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>357013</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1890,10 +1953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1931,7 +1994,7 @@
         <v>20180620</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1939,7 +2002,7 @@
         <v>20180629</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="45">
@@ -1947,7 +2010,7 @@
         <v>20180702</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="45">
@@ -1955,7 +2018,7 @@
         <v>20180706</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="105">
@@ -1963,7 +2026,7 @@
         <v>20180707</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30">
@@ -1971,7 +2034,7 @@
         <v>20180714</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="45">
@@ -1979,7 +2042,7 @@
         <v>20180723</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30">
@@ -1987,7 +2050,7 @@
         <v>20180725</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="75">
@@ -1995,7 +2058,7 @@
         <v>20181011</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="105">
@@ -2003,7 +2066,7 @@
         <v>20181030</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="105">
@@ -2011,7 +2074,7 @@
         <v>20181031</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="105">
@@ -2019,7 +2082,7 @@
         <v>20181105</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="60">
@@ -2027,7 +2090,7 @@
         <v>20181107</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="120">
@@ -2035,7 +2098,7 @@
         <v>20181129</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="315">
@@ -2043,7 +2106,7 @@
         <v>20181205</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="45">
@@ -2051,7 +2114,7 @@
         <v>20181208</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="225">
@@ -2059,7 +2122,7 @@
         <v>20181228</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="120">
@@ -2067,7 +2130,7 @@
         <v>20181228</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="45">
@@ -2075,7 +2138,7 @@
         <v>20180213</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="90">
@@ -2083,7 +2146,7 @@
         <v>20180221</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="105">
@@ -2091,7 +2154,7 @@
         <v>20180222</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="75">
@@ -2099,7 +2162,15 @@
         <v>20180227</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="120">
+      <c r="A26" s="1">
+        <v>20180228</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2110,10 +2181,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K77"/>
+  <dimension ref="A1:K79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2199,10 +2270,10 @@
     </row>
     <row r="4" spans="1:11" ht="120">
       <c r="A4" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>24</v>
+        <v>173</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>14</v>
@@ -2213,19 +2284,21 @@
       <c r="E4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="6"/>
+      <c r="F4" s="14" t="s">
+        <v>178</v>
+      </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" ht="45">
+    <row r="5" spans="1:11" ht="60">
       <c r="A5" s="5" t="s">
-        <v>27</v>
+        <v>172</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>25</v>
+        <v>174</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>14</v>
@@ -2236,7 +2309,9 @@
       <c r="E5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="6"/>
+      <c r="F5" s="14" t="s">
+        <v>177</v>
+      </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -2245,73 +2320,85 @@
     </row>
     <row r="6" spans="1:11" ht="60">
       <c r="A6" s="5" t="s">
-        <v>6</v>
+        <v>175</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>9</v>
+        <v>176</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>179</v>
+      </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" ht="75">
+    <row r="7" spans="1:11" ht="60">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>26</v>
+        <v>180</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>21</v>
-      </c>
+      <c r="D7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" ht="45">
-      <c r="A8" s="6" t="s">
-        <v>29</v>
+    <row r="8" spans="1:11" ht="75">
+      <c r="A8" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+    <row r="9" spans="1:11" ht="45">
+      <c r="A9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -2477,19 +2564,11 @@
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="1:11" ht="30">
-      <c r="A22" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>31</v>
-      </c>
+    <row r="22" spans="1:11">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -2498,18 +2577,18 @@
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
     </row>
-    <row r="23" spans="1:11" ht="75">
+    <row r="23" spans="1:11" ht="30">
       <c r="A23" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
@@ -2519,17 +2598,19 @@
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
     </row>
-    <row r="24" spans="1:11" ht="30">
-      <c r="A24" s="6" t="s">
-        <v>29</v>
+    <row r="24" spans="1:11" ht="75">
+      <c r="A24" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
@@ -2538,19 +2619,17 @@
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
     </row>
-    <row r="25" spans="1:11" ht="165">
+    <row r="25" spans="1:11" ht="30">
       <c r="A25" s="6" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>42</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
@@ -2559,59 +2638,61 @@
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="1:11" ht="90">
-      <c r="A26" s="5" t="s">
-        <v>6</v>
+    <row r="26" spans="1:11" ht="165">
+      <c r="A26" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
     </row>
-    <row r="27" spans="1:11" ht="45">
-      <c r="A27" s="6" t="s">
-        <v>52</v>
+    <row r="27" spans="1:11" ht="90">
+      <c r="A27" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
+        <v>42</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
     </row>
-    <row r="28" spans="1:11" ht="60">
-      <c r="A28" s="5" t="s">
-        <v>54</v>
+    <row r="28" spans="1:11" ht="45">
+      <c r="A28" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -2622,15 +2703,15 @@
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
     </row>
-    <row r="29" spans="1:11" ht="45">
-      <c r="A29" s="6" t="s">
-        <v>29</v>
+    <row r="29" spans="1:11" ht="60">
+      <c r="A29" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
@@ -2641,274 +2722,280 @@
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
     </row>
-    <row r="30" spans="1:11" ht="150">
-      <c r="A30" s="5" t="s">
-        <v>6</v>
+    <row r="30" spans="1:11" ht="45">
+      <c r="A30" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>152</v>
+        <v>57</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>150</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
     </row>
-    <row r="31" spans="1:11" ht="45">
+    <row r="31" spans="1:11" ht="150">
       <c r="A31" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>67</v>
+        <v>150</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
+        <v>62</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
     </row>
-    <row r="32" spans="1:11" ht="75">
+    <row r="32" spans="1:11" ht="45">
       <c r="A32" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>153</v>
+        <v>64</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-    </row>
-    <row r="33" spans="1:11" ht="60">
+        <v>66</v>
+      </c>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+    </row>
+    <row r="33" spans="1:11" ht="75">
       <c r="A33" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>76</v>
+        <v>151</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H33" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
+        <v>147</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
     </row>
     <row r="34" spans="1:11" ht="60">
       <c r="A34" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="9"/>
-    </row>
-    <row r="35" spans="1:11" ht="45">
+        <v>74</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+    </row>
+    <row r="35" spans="1:11" ht="60">
       <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C35" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
-    </row>
-    <row r="36" spans="1:11" ht="135">
+      <c r="C35" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+    </row>
+    <row r="36" spans="1:11" ht="45">
       <c r="A36" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>115</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
-      <c r="I36" s="5" t="s">
-        <v>117</v>
-      </c>
+      <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
     </row>
-    <row r="37" spans="1:11" ht="45">
+    <row r="37" spans="1:11" ht="135">
       <c r="A37" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="9" t="s">
-        <v>89</v>
+      <c r="B37" s="5" t="s">
+        <v>114</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>97</v>
+        <v>83</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>113</v>
       </c>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
+      <c r="I37" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
     </row>
-    <row r="38" spans="1:11" ht="60">
+    <row r="38" spans="1:11" ht="45">
       <c r="A38" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E38" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="F38" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="D38" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="F38" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="G38" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="H38" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="I38" s="11"/>
-      <c r="J38" s="10"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
       <c r="K38" s="5"/>
     </row>
-    <row r="39" spans="1:11" ht="75">
+    <row r="39" spans="1:11" ht="60">
       <c r="A39" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="C39" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="I39" s="11"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="5"/>
+    </row>
+    <row r="40" spans="1:11" ht="75">
+      <c r="A40" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E40" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="F40" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="G40" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="F39" s="11" t="s">
+      <c r="H40" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="G39" s="11" t="s">
+      <c r="I40" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="H39" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="I39" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-    </row>
-    <row r="40" spans="1:11">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
-      <c r="K40" s="10"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="10"/>
@@ -3170,44 +3257,34 @@
       <c r="J60" s="10"/>
       <c r="K60" s="10"/>
     </row>
-    <row r="61" spans="1:11" ht="60">
-      <c r="A61" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E61" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5"/>
-      <c r="H61" s="5"/>
-      <c r="I61" s="5"/>
-      <c r="J61" s="5"/>
-      <c r="K61" s="5"/>
-    </row>
-    <row r="62" spans="1:11" ht="30">
+    <row r="61" spans="1:11">
+      <c r="A61" s="10"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="10"/>
+      <c r="G61" s="10"/>
+      <c r="H61" s="10"/>
+      <c r="I61" s="10"/>
+      <c r="J61" s="10"/>
+      <c r="K61" s="10"/>
+    </row>
+    <row r="62" spans="1:11" ht="60">
       <c r="A62" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B62" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>119</v>
+      <c r="B62" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>108</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
@@ -3220,16 +3297,18 @@
       <c r="A63" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="E63" s="5"/>
+      <c r="B63" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D63" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="E63" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
@@ -3242,12 +3321,14 @@
         <v>6</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D64" s="5"/>
+        <v>121</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>122</v>
+      </c>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
@@ -3261,9 +3342,11 @@
         <v>6</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C65" s="5"/>
+        <v>124</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>125</v>
+      </c>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
@@ -3273,19 +3356,15 @@
       <c r="J65" s="5"/>
       <c r="K65" s="5"/>
     </row>
-    <row r="66" spans="1:11" ht="45">
+    <row r="66" spans="1:11" ht="30">
       <c r="A66" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>131</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
       <c r="G66" s="5"/>
@@ -3296,20 +3375,18 @@
     </row>
     <row r="67" spans="1:11" ht="45">
       <c r="A67" s="5" t="s">
-        <v>134</v>
+        <v>6</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>16</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E67" s="5"/>
       <c r="F67" s="5"/>
       <c r="G67" s="5"/>
       <c r="H67" s="5"/>
@@ -3317,18 +3394,22 @@
       <c r="J67" s="5"/>
       <c r="K67" s="5"/>
     </row>
-    <row r="68" spans="1:11" ht="30">
-      <c r="A68" s="6" t="s">
-        <v>135</v>
+    <row r="68" spans="1:11" ht="45">
+      <c r="A68" s="5" t="s">
+        <v>132</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
+        <v>130</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
       <c r="H68" s="5"/>
@@ -3336,19 +3417,17 @@
       <c r="J68" s="5"/>
       <c r="K68" s="5"/>
     </row>
-    <row r="69" spans="1:11" ht="45">
-      <c r="A69" s="5" t="s">
-        <v>6</v>
+    <row r="69" spans="1:11" ht="30">
+      <c r="A69" s="6" t="s">
+        <v>133</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>140</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="D69" s="5"/>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
       <c r="G69" s="5"/>
@@ -3362,13 +3441,13 @@
         <v>6</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
@@ -3378,18 +3457,18 @@
       <c r="J70" s="5"/>
       <c r="K70" s="5"/>
     </row>
-    <row r="71" spans="1:11" ht="75">
+    <row r="71" spans="1:11" ht="45">
       <c r="A71" s="5" t="s">
-        <v>147</v>
+        <v>6</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
@@ -3399,17 +3478,19 @@
       <c r="J71" s="5"/>
       <c r="K71" s="5"/>
     </row>
-    <row r="72" spans="1:11" ht="30">
+    <row r="72" spans="1:11" ht="75">
       <c r="A72" s="5" t="s">
-        <v>6</v>
+        <v>145</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="D72" s="5"/>
+        <v>146</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>144</v>
+      </c>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
       <c r="G72" s="5"/>
@@ -3423,14 +3504,12 @@
         <v>6</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>157</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="D73" s="5"/>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
@@ -3439,18 +3518,18 @@
       <c r="J73" s="5"/>
       <c r="K73" s="5"/>
     </row>
-    <row r="74" spans="1:11" ht="45">
+    <row r="74" spans="1:11" ht="30">
       <c r="A74" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>129</v>
+        <v>156</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
@@ -3460,18 +3539,18 @@
       <c r="J74" s="5"/>
       <c r="K74" s="5"/>
     </row>
-    <row r="75" spans="1:11" ht="60">
+    <row r="75" spans="1:11" ht="45">
       <c r="A75" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>163</v>
+        <v>127</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
@@ -3481,18 +3560,18 @@
       <c r="J75" s="5"/>
       <c r="K75" s="5"/>
     </row>
-    <row r="76" spans="1:11" ht="90">
+    <row r="76" spans="1:11" ht="60">
       <c r="A76" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
@@ -3502,18 +3581,18 @@
       <c r="J76" s="5"/>
       <c r="K76" s="5"/>
     </row>
-    <row r="77" spans="1:11" ht="45">
+    <row r="77" spans="1:11" ht="90">
       <c r="A77" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E77" s="5"/>
       <c r="F77" s="5"/>
@@ -3522,6 +3601,48 @@
       <c r="I77" s="5"/>
       <c r="J77" s="5"/>
       <c r="K77" s="5"/>
+    </row>
+    <row r="78" spans="1:11" ht="45">
+      <c r="A78" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+      <c r="G78" s="5"/>
+      <c r="H78" s="5"/>
+      <c r="I78" s="5"/>
+      <c r="J78" s="5"/>
+      <c r="K78" s="5"/>
+    </row>
+    <row r="79" spans="1:11" ht="45">
+      <c r="A79" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
+      <c r="H79" s="5"/>
+      <c r="I79" s="5"/>
+      <c r="J79" s="5"/>
+      <c r="K79" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Support to export x_t
Support to export x_t
</commit_message>
<xml_diff>
--- a/修改日志.xlsx
+++ b/修改日志.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="184">
   <si>
     <t>日期</t>
   </si>
@@ -1350,6 +1350,10 @@
     <t>bugfix : 
 pick edge\pick face\pick vertex
 问题来自于0312的代码修改</t>
+  </si>
+  <si>
+    <t>新增：
+支持x_t导出</t>
   </si>
 </sst>
 </file>
@@ -1991,10 +1995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2173,7 +2177,7 @@
     </row>
     <row r="22" spans="1:2" ht="45">
       <c r="A22" s="1">
-        <v>20180213</v>
+        <v>20190213</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>157</v>
@@ -2181,7 +2185,7 @@
     </row>
     <row r="23" spans="1:2" ht="90">
       <c r="A23" s="1">
-        <v>20180221</v>
+        <v>20190221</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>163</v>
@@ -2189,7 +2193,7 @@
     </row>
     <row r="24" spans="1:2" ht="105">
       <c r="A24" s="1">
-        <v>20180222</v>
+        <v>20190222</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>167</v>
@@ -2197,7 +2201,7 @@
     </row>
     <row r="25" spans="1:2" ht="75">
       <c r="A25" s="1">
-        <v>20180227</v>
+        <v>20190227</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>168</v>
@@ -2205,7 +2209,7 @@
     </row>
     <row r="26" spans="1:2" ht="120">
       <c r="A26" s="1">
-        <v>20180228</v>
+        <v>20190228</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>171</v>
@@ -2213,7 +2217,7 @@
     </row>
     <row r="27" spans="1:2" ht="45">
       <c r="A27" s="1">
-        <v>20180312</v>
+        <v>20190312</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>181</v>
@@ -2221,10 +2225,18 @@
     </row>
     <row r="28" spans="1:2" ht="45">
       <c r="A28" s="1">
-        <v>20180313</v>
+        <v>20190313</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>182</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="30">
+      <c r="A29" s="1">
+        <v>20190505</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Support to export dwg\dxf
Support to export dwg\dxf
</commit_message>
<xml_diff>
--- a/修改日志.xlsx
+++ b/修改日志.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="185">
   <si>
     <t>日期</t>
   </si>
@@ -1354,6 +1354,10 @@
   <si>
     <t>新增：
 支持x_t导出</t>
+  </si>
+  <si>
+    <t>新增：
+支持dwg\dxf导出</t>
   </si>
 </sst>
 </file>
@@ -1995,10 +1999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2237,6 +2241,14 @@
       </c>
       <c r="B29" s="3" t="s">
         <v>183</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="30">
+      <c r="A30" s="1">
+        <v>20190507</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
assembly export mode change
For single body model, assembly and part export mode will generate the same result
</commit_message>
<xml_diff>
--- a/修改日志.xlsx
+++ b/修改日志.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="修改记录" sheetId="1" r:id="rId1"/>
@@ -1576,11 +1576,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2082,8 +2082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2373,17 +2373,17 @@
       <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" spans="1:11" ht="70.5" customHeight="1">
       <c r="A2" s="5" t="s">
@@ -3848,8 +3848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3864,7 +3864,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>190</v>
       </c>
       <c r="B2" t="s">
@@ -3872,7 +3872,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>192</v>
       </c>
       <c r="B3" t="s">
@@ -3880,7 +3880,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>193</v>
       </c>
       <c r="B4" t="s">
@@ -3888,7 +3888,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="30">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>194</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -3896,7 +3896,7 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>197</v>
       </c>
       <c r="B6" t="s">

</xml_diff>

<commit_message>
bugfix - 2D Drawing zoom to extent (AutoCAD Ok but DraftSight NG)
</commit_message>
<xml_diff>
--- a/修改日志.xlsx
+++ b/修改日志.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="213">
   <si>
     <t>日期</t>
   </si>
@@ -1612,6 +1612,11 @@
 1. Some entities cannot be saved to SAT if back-saving to R16
 2. 2D Drawing zoom to extent
 3. 2D Drawing text size</t>
+  </si>
+  <si>
+    <t>修改：
+bugfixs
+1. 2D Drawing zoom to extent (AutoCAD Ok but DraftSight NG)</t>
   </si>
 </sst>
 </file>
@@ -2261,10 +2266,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2545,6 +2550,14 @@
         <v>211</v>
       </c>
     </row>
+    <row r="35" spans="1:2" ht="45">
+      <c r="A35" s="1">
+        <v>20191023</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2555,8 +2568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K81"/>
   <sheetViews>
-    <sheetView topLeftCell="B75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+    <sheetView topLeftCell="B63" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
bugfix for 2D Drawing module
1. filter out all bodies from the input SAT file
2. apply the transformation to each body
</commit_message>
<xml_diff>
--- a/修改日志.xlsx
+++ b/修改日志.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="214">
   <si>
     <t>日期</t>
   </si>
@@ -1618,11 +1618,17 @@
 bugfixs
 1. 2D Drawing zoom to extent (AutoCAD Ok but DraftSight NG)</t>
   </si>
+  <si>
+    <t>修改：
+bugfix for 2D Drawing module
+1. filter out all bodies from the input SAT file
+2. apply the transformation to each body</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -1770,15 +1776,18 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="好" xfId="2" builtinId="26"/>
-    <cellStyle name="注释" xfId="1" builtinId="10"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1980,7 +1989,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2022,7 +2031,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2057,7 +2066,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2266,10 +2275,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2556,6 +2565,14 @@
       </c>
       <c r="B35" s="3" t="s">
         <v>212</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="60">
+      <c r="A36" s="1">
+        <v>20191208</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>